<commit_message>
table 2 outcome in excel
</commit_message>
<xml_diff>
--- a/analysis/output/table2.xlsx
+++ b/analysis/output/table2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -65,6 +65,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -108,12 +111,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,14 +145,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
@@ -474,87 +494,106 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="39.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" ht="22" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>7.5263</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>7.29</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>5.9714</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" ht="29" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="B4" s="4">
+        <v>0.54259176664198205</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.437214006143746</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.6216333653706501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="25" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="24" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="B6" s="4">
+        <v>143.312699796011</v>
+      </c>
+      <c r="C6" s="4">
+        <v>34.518457974094403</v>
+      </c>
+      <c r="D6" s="4">
+        <v>128.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="27" customHeight="1">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>11.771689796893099</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>10.820666221578501</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>60.282872831796602</v>
       </c>
     </row>

</xml_diff>